<commit_message>
adjusted some stuff and completed formula stuff
</commit_message>
<xml_diff>
--- a/Medallion prices over time.xlsx
+++ b/Medallion prices over time.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donti\Documents\GitHub\DS3001-Case-4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arun\Documents\GitHub\DS3001-Case-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16440" windowHeight="4757"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16440" windowHeight="4755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -302,91 +302,91 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>26</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>28</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>29</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>30</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>31</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>34</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>35</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1585,16 +1585,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.07421875" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>41640</v>
       </c>
@@ -1614,10 +1614,10 @@
         <v>967500</v>
       </c>
       <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>41671</v>
       </c>
@@ -1626,10 +1626,10 @@
         <v>981500</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>41699</v>
       </c>
@@ -1638,10 +1638,10 @@
         <v>1011666.6666666666</v>
       </c>
       <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>41730</v>
       </c>
@@ -1650,10 +1650,10 @@
         <v>1013875</v>
       </c>
       <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>41760</v>
       </c>
@@ -1662,10 +1662,10 @@
         <v>993571.42857142852</v>
       </c>
       <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>41791</v>
       </c>
@@ -1674,10 +1674,10 @@
         <v>989166.66666666663</v>
       </c>
       <c r="C7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>41821</v>
       </c>
@@ -1686,10 +1686,10 @@
         <v>1001250</v>
       </c>
       <c r="C8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>41852</v>
       </c>
@@ -1698,10 +1698,10 @@
         <v>925000</v>
       </c>
       <c r="C9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>41883</v>
       </c>
@@ -1710,10 +1710,10 @@
         <v>900000</v>
       </c>
       <c r="C10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>41913</v>
       </c>
@@ -1722,10 +1722,10 @@
         <v>871666.66666666663</v>
       </c>
       <c r="C11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>41944</v>
       </c>
@@ -1734,10 +1734,10 @@
         <v>840000</v>
       </c>
       <c r="C12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>41974</v>
       </c>
@@ -1746,10 +1746,10 @@
         <v>805000</v>
       </c>
       <c r="C13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>42005</v>
       </c>
@@ -1758,10 +1758,10 @@
         <v>800000</v>
       </c>
       <c r="C14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42064</v>
       </c>
@@ -1769,10 +1769,10 @@
         <v>800000</v>
       </c>
       <c r="C15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>42125</v>
       </c>
@@ -1780,10 +1780,10 @@
         <v>700000</v>
       </c>
       <c r="C16">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>42156</v>
       </c>
@@ -1792,10 +1792,10 @@
         <v>767250</v>
       </c>
       <c r="C17">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>42186</v>
       </c>
@@ -1804,10 +1804,10 @@
         <v>603000</v>
       </c>
       <c r="C18">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>42217</v>
       </c>
@@ -1816,10 +1816,10 @@
         <v>717500</v>
       </c>
       <c r="C19">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>42248</v>
       </c>
@@ -1828,10 +1828,10 @@
         <v>715000</v>
       </c>
       <c r="C20">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>42278</v>
       </c>
@@ -1840,10 +1840,10 @@
         <v>675000</v>
       </c>
       <c r="C21">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>42339</v>
       </c>
@@ -1852,10 +1852,10 @@
         <v>715000</v>
       </c>
       <c r="C22">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>42430</v>
       </c>
@@ -1864,10 +1864,10 @@
         <v>550000</v>
       </c>
       <c r="C23">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>42461</v>
       </c>
@@ -1876,10 +1876,10 @@
         <v>615000</v>
       </c>
       <c r="C24">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>42491</v>
       </c>
@@ -1888,10 +1888,10 @@
         <v>550000</v>
       </c>
       <c r="C25">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>42522</v>
       </c>
@@ -1900,10 +1900,10 @@
         <v>571785.71428571432</v>
       </c>
       <c r="C26">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>42552</v>
       </c>
@@ -1912,13 +1912,13 @@
         <v>585000</v>
       </c>
       <c r="C27">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F27" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>42583</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>596000</v>
       </c>
       <c r="C28">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>5</v>
@@ -1936,7 +1936,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>42675</v>
       </c>
@@ -1945,13 +1945,13 @@
         <v>500000</v>
       </c>
       <c r="C29">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F29" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>42705</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>543333.33333333337</v>
       </c>
       <c r="C30">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>7</v>

</xml_diff>